<commit_message>
Adicionando teste de mesa em excel
</commit_message>
<xml_diff>
--- a/bancoDeDados/senai_roman_desafio_bd_importacao.xlsx
+++ b/bancoDeDados/senai_roman_desafio_bd_importacao.xlsx
@@ -2,14 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\senai_roman_desafio_projectmanagement\bancoDeDados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="TIPOSUSUARIO" sheetId="6" r:id="rId1"/>
+    <sheet name="EQUIPES" sheetId="11" r:id="rId2"/>
+    <sheet name="USUARIOS" sheetId="7" r:id="rId3"/>
+    <sheet name="TEMAS" sheetId="9" r:id="rId4"/>
+    <sheet name="PROJETOS" sheetId="12" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +27,134 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>fernando@email.com</t>
+  </si>
+  <si>
+    <t>helena@email.com</t>
+  </si>
+  <si>
+    <t>admin12345</t>
+  </si>
+  <si>
+    <t>saulo@email.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>Saulo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TIPO_USUARIO</t>
+  </si>
+  <si>
+    <t>PROFESSOR</t>
+  </si>
+  <si>
+    <t>EQUIPES</t>
+  </si>
+  <si>
+    <t>DESENVOLVIMENTO</t>
+  </si>
+  <si>
+    <t>REDES</t>
+  </si>
+  <si>
+    <t>MULTIMÍDIA</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>SENHA</t>
+  </si>
+  <si>
+    <t>TIPOUSUARIO_ID</t>
+  </si>
+  <si>
+    <t>EQUIPE_ID</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>barbara@email.com</t>
+  </si>
+  <si>
+    <t>gabriel@email.com</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>TEMA</t>
+  </si>
+  <si>
+    <t>ATIVO</t>
+  </si>
+  <si>
+    <t>HQs</t>
+  </si>
+  <si>
+    <t>Gestão</t>
+  </si>
+  <si>
+    <t>Finanças</t>
+  </si>
+  <si>
+    <t>DESCRICAO</t>
+  </si>
+  <si>
+    <t>TEMA_ID</t>
+  </si>
+  <si>
+    <t>Personagens</t>
+  </si>
+  <si>
+    <t>Carfel</t>
+  </si>
+  <si>
+    <t>Finaça de mesa</t>
+  </si>
+  <si>
+    <t>Projeto para listar personagens</t>
+  </si>
+  <si>
+    <t>Projeto para controle de ponto digital</t>
+  </si>
+  <si>
+    <t>Projeto para gerenciar finanças pessoais</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +162,84 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -45,18 +247,216 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -69,7 +469,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +514,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +549,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +731,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="29">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="31">
+        <v>12345</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="31">
+        <v>12345</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="31">
+        <v>12345</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="31">
+        <v>12345</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="32">
+        <v>12345</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="16"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>5</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="45">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionando script de manipulacao DML
</commit_message>
<xml_diff>
--- a/bancoDeDados/senai_roman_desafio_bd_importacao.xlsx
+++ b/bancoDeDados/senai_roman_desafio_bd_importacao.xlsx
@@ -69,9 +69,6 @@
     <t>PROFESSOR</t>
   </si>
   <si>
-    <t>EQUIPES</t>
-  </si>
-  <si>
     <t>DESENVOLVIMENTO</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Carfel</t>
   </si>
   <si>
-    <t>Finaça de mesa</t>
-  </si>
-  <si>
     <t>Projeto para listar personagens</t>
   </si>
   <si>
@@ -148,6 +142,12 @@
   </si>
   <si>
     <t>Projeto para gerenciar finanças pessoais</t>
+  </si>
+  <si>
+    <t>EQUIPE</t>
+  </si>
+  <si>
+    <t>Finança de mesa</t>
   </si>
 </sst>
 </file>
@@ -791,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +807,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -846,19 +846,19 @@
         <v>10</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="35" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -926,10 +926,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="31">
         <v>12345</v>
@@ -946,10 +946,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="31">
         <v>12345</v>
@@ -1018,10 +1018,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="21">
         <v>1</v>
@@ -1040,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="22">
         <v>0</v>
@@ -1073,7 +1073,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1083,13 +1083,13 @@
         <v>10</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1097,10 +1097,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="40">
         <v>1</v>
@@ -1111,10 +1111,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="40">
         <v>2</v>
@@ -1125,10 +1125,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="45">
         <v>3</v>

</xml_diff>